<commit_message>
update report name in defintion tab
</commit_message>
<xml_diff>
--- a/OpenResultsData/Docs/ORD_Data_Spec.xlsx
+++ b/OpenResultsData/Docs/ORD_Data_Spec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -488,7 +488,7 @@
     <t xml:space="preserve">Per Sample Exceedance Probability Table (PSEPT)</t>
   </si>
   <si>
-    <t xml:space="preserve">Error Log (ELOG)</t>
+    <t xml:space="preserve">ExposureSummary (EXPSUM)</t>
   </si>
   <si>
     <t xml:space="preserve">Only contains rows where Loss &gt; 0</t>
@@ -518,6 +518,9 @@
     <t xml:space="preserve">Existing amended table</t>
   </si>
   <si>
+    <t xml:space="preserve">New Table</t>
+  </si>
+  <si>
     <t xml:space="preserve">EventId</t>
   </si>
   <si>
@@ -1361,27 +1364,6 @@
     <t xml:space="preserve">For exposure</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ELOG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,EXPSUM</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Account number</t>
   </si>
   <si>
@@ -1391,25 +1373,7 @@
     <t xml:space="preserve">Peril code</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ELOG,REJEXP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,EXPSUM</t>
-    </r>
+    <t xml:space="preserve">ELOG,REJEXP,EXPSUM</t>
   </si>
   <si>
     <t xml:space="preserve">Error message</t>
@@ -1753,7 +1717,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1880,12 +1844,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2314,15 +2272,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2342,18 +2300,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2385,7 +2343,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2490,7 +2448,7 @@
   </sheetPr>
   <dimension ref="B1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2747,7 +2705,7 @@
   </sheetPr>
   <dimension ref="B1:H56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -3420,8 +3378,8 @@
   </sheetPr>
   <dimension ref="B1:DC53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CO1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CU15" activeCellId="0" sqref="CU15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3721,300 +3679,300 @@
         <v>134</v>
       </c>
       <c r="CU14" s="46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="47" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C15" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="J15" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="K15" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="L15" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="N15" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="O15" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="P15" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q15" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="R15" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="S15" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="T15" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="U15" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="V15" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="W15" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="X15" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y15" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z15" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA15" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB15" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC15" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE15" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF15" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG15" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH15" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI15" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ15" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK15" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL15" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="AM15" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN15" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="AO15" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="AP15" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="J15" s="48" t="s">
+      <c r="AQ15" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="AS15" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="AT15" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU15" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="K15" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="L15" s="49" t="s">
+      <c r="AV15" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="AW15" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="AX15" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="AY15" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="AZ15" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="BA15" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB15" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC15" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="BE15" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="BF15" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="BG15" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="BH15" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="BI15" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="BJ15" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK15" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="BL15" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM15" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="BN15" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="BO15" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="BP15" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="BQ15" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR15" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="BS15" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT15" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="BU15" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="BV15" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="BW15" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="BX15" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY15" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="BZ15" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="CB15" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="CC15" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="CD15" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="CE15" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="CF15" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="CG15" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="CI15" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="CJ15" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="CK15" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="CL15" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="CM15" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="CO15" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP15" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="N15" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="O15" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="P15" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q15" s="48" t="s">
-        <v>143</v>
-      </c>
-      <c r="R15" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="S15" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="T15" s="50" t="s">
-        <v>146</v>
-      </c>
-      <c r="U15" s="50" t="s">
-        <v>147</v>
-      </c>
-      <c r="V15" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="W15" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="X15" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="Y15" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z15" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA15" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB15" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC15" s="49" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE15" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF15" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="AG15" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="AH15" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="AI15" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="AJ15" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="AK15" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="AL15" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="AM15" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="AN15" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO15" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP15" s="48" t="s">
+      <c r="CQ15" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="CR15" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="CS15" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="AQ15" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS15" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="AT15" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU15" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV15" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="AW15" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="AX15" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="AY15" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="AZ15" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="BA15" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="BB15" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="BC15" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="BE15" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="BF15" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="BG15" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="BH15" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="BI15" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="BJ15" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="BK15" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="BL15" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="BM15" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="BN15" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="BO15" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="BP15" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="BQ15" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="BR15" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="BS15" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="BT15" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="BU15" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="BV15" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="BW15" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="BX15" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="BY15" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="BZ15" s="49" t="s">
-        <v>155</v>
-      </c>
-      <c r="CB15" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="CC15" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="CD15" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="CE15" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="CF15" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="CG15" s="51" t="s">
-        <v>164</v>
-      </c>
-      <c r="CI15" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="CJ15" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="CK15" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="CL15" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="CM15" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="CO15" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="CP15" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="CQ15" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="CR15" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="CS15" s="49" t="s">
-        <v>138</v>
-      </c>
       <c r="CU15" s="47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CV15" s="48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CW15" s="48" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CX15" s="48" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CY15" s="48" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CZ15" s="48" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="DA15" s="48" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="DB15" s="48" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="DC15" s="49" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,7 +5750,7 @@
       <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="59" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="59" width="12"/>
@@ -5855,536 +5813,536 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="E2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="G2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="H2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="J2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="K2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="M2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="M2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="N2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="Q2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="S2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="S2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="T2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="V2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="W2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="Y2" s="61" t="s">
-        <v>177</v>
-      </c>
       <c r="Z2" s="61" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="59" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J3" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M3" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="P3" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="S3" s="59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="T3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="V3" s="59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Y3" s="59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Z3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="59" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B4" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="K4" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="59" t="s">
+      <c r="M4" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="N4" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="H4" s="59" t="s">
+      <c r="P4" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q4" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="J4" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="K4" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="M4" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="N4" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="P4" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q4" s="59" t="s">
-        <v>179</v>
-      </c>
       <c r="S4" s="59" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="T4" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="V4" s="59" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="W4" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Y4" s="59" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Z4" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G5" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J5" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="M5" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="K5" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="M5" s="59" t="s">
-        <v>141</v>
-      </c>
       <c r="N5" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="P5" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q5" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="P5" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q5" s="59" t="s">
-        <v>179</v>
-      </c>
       <c r="S5" s="59" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="T5" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="V5" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="W5" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="V5" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="W5" s="59" t="s">
-        <v>179</v>
-      </c>
       <c r="Y5" s="59" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Z5" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="59" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H6" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J6" s="59" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K6" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M6" s="59" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N6" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P6" s="59" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q6" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="T6" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="V6" s="59" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="W6" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Y6" s="59" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Z6" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="59" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H7" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J7" s="59" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K7" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P7" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q7" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="V7" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="Q7" s="59" t="s">
-        <v>180</v>
-      </c>
-      <c r="V7" s="59" t="s">
-        <v>138</v>
-      </c>
       <c r="W7" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Y7" s="59" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Z7" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="59" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G8" s="59" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H8" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J8" s="59" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K8" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G9" s="59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H9" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J9" s="59" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K9" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="59" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H10" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J10" s="59" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K10" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D11" s="59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H11" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J11" s="59" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K11" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>141</v>
-      </c>
       <c r="E12" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="G12" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="H12" s="59" t="s">
-        <v>179</v>
-      </c>
       <c r="J12" s="59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K12" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="59" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D13" s="59" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E13" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H13" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J13" s="59" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K13" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="59" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H14" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="59" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="59" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="59" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="59" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -6417,8 +6375,8 @@
   </sheetPr>
   <dimension ref="B1:I157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C117" activeCellId="0" sqref="C117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E108" activeCellId="0" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6437,7 +6395,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="62" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6448,10 +6406,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="64" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6463,25 +6421,25 @@
         <v>31</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E7" s="65" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F7" s="65" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G7" s="66" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H7" s="65" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I7" s="66" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,19 +6447,19 @@
         <v>38</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H8" s="9"/>
     </row>
@@ -6510,22 +6468,22 @@
         <v>38</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6533,19 +6491,19 @@
         <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H10" s="9"/>
     </row>
@@ -6554,19 +6512,19 @@
         <v>38</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H11" s="9"/>
     </row>
@@ -6581,13 +6539,13 @@
         <v>6</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H12" s="9"/>
     </row>
@@ -6596,16 +6554,16 @@
         <v>38</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="11" t="s">
@@ -6617,16 +6575,16 @@
         <v>38</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="11" t="s">
@@ -6638,22 +6596,22 @@
         <v>38</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6661,19 +6619,19 @@
         <v>38</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H16" s="9"/>
     </row>
@@ -6682,19 +6640,19 @@
         <v>38</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H17" s="9"/>
     </row>
@@ -6709,13 +6667,13 @@
         <v>6</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>42</v>
@@ -6726,19 +6684,19 @@
         <v>38</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H19" s="9"/>
     </row>
@@ -6747,19 +6705,19 @@
         <v>38</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H20" s="9"/>
     </row>
@@ -6768,19 +6726,19 @@
         <v>38</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H21" s="9"/>
     </row>
@@ -6789,19 +6747,19 @@
         <v>38</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H22" s="9"/>
     </row>
@@ -6810,19 +6768,19 @@
         <v>38</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H23" s="9"/>
     </row>
@@ -6831,17 +6789,17 @@
         <v>38</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F24" s="67"/>
       <c r="G24" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="11" t="s">
@@ -6853,17 +6811,17 @@
         <v>38</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F25" s="67"/>
       <c r="G25" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="11" t="s">
@@ -6881,13 +6839,13 @@
         <v>6</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>42</v>
@@ -6898,19 +6856,19 @@
         <v>91</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H27" s="36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I27" s="11" t="s">
         <v>42</v>
@@ -6921,19 +6879,19 @@
         <v>91</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H28" s="36" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>42</v>
@@ -6944,19 +6902,19 @@
         <v>91</v>
       </c>
       <c r="C29" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>42</v>
@@ -6967,17 +6925,17 @@
         <v>38</v>
       </c>
       <c r="C30" s="67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F30" s="63"/>
       <c r="G30" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="11" t="s">
@@ -6989,17 +6947,17 @@
         <v>38</v>
       </c>
       <c r="C31" s="67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="67" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F31" s="63"/>
       <c r="G31" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="11" t="s">
@@ -7011,16 +6969,16 @@
         <v>38</v>
       </c>
       <c r="C32" s="67" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="11" t="s">
@@ -7032,19 +6990,19 @@
         <v>38</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D33" s="68" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="68" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G33" s="36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H33" s="69" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I33" s="36" t="s">
         <v>42</v>
@@ -7055,16 +7013,16 @@
         <v>38</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="68" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H34" s="36"/>
       <c r="I34" s="36" t="s">
@@ -7076,16 +7034,16 @@
         <v>38</v>
       </c>
       <c r="C35" s="67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D35" s="68" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H35" s="36"/>
       <c r="I35" s="36" t="s">
@@ -7097,20 +7055,20 @@
         <v>38</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D36" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F36" s="67"/>
       <c r="G36" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I36" s="35" t="s">
         <v>42</v>
@@ -7121,20 +7079,20 @@
         <v>38</v>
       </c>
       <c r="C37" s="67" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D37" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="67" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F37" s="67"/>
       <c r="G37" s="35" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H37" s="35" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I37" s="35" t="s">
         <v>42</v>
@@ -7145,20 +7103,20 @@
         <v>38</v>
       </c>
       <c r="C38" s="67" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D38" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F38" s="67"/>
       <c r="G38" s="35" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I38" s="67" t="s">
         <v>42</v>
@@ -7169,18 +7127,18 @@
         <v>86</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D39" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F39" s="67"/>
       <c r="G39" s="35"/>
       <c r="H39" s="35" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I39" s="67" t="s">
         <v>42</v>
@@ -7191,20 +7149,20 @@
         <v>86</v>
       </c>
       <c r="C40" s="67" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D40" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="70" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F40" s="70"/>
       <c r="G40" s="35" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I40" s="11" t="s">
         <v>42</v>
@@ -7215,17 +7173,17 @@
         <v>86</v>
       </c>
       <c r="C41" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D41" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E41" s="70" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F41" s="70"/>
       <c r="G41" s="35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="11" t="s">
@@ -7237,19 +7195,19 @@
         <v>86</v>
       </c>
       <c r="C42" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H42" s="9"/>
     </row>
@@ -7258,16 +7216,16 @@
         <v>86</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="11" t="s">
@@ -7279,19 +7237,19 @@
         <v>86</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>42</v>
@@ -7302,19 +7260,19 @@
         <v>86</v>
       </c>
       <c r="C45" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H45" s="9"/>
     </row>
@@ -7323,17 +7281,17 @@
         <v>86</v>
       </c>
       <c r="C46" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F46" s="67"/>
       <c r="G46" s="35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H46" s="35"/>
       <c r="I46" s="67" t="s">
@@ -7345,20 +7303,20 @@
         <v>86</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="70" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F47" s="67"/>
       <c r="G47" s="35" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H47" s="35" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I47" s="67" t="s">
         <v>42</v>
@@ -7369,17 +7327,17 @@
         <v>86</v>
       </c>
       <c r="C48" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F48" s="67"/>
       <c r="G48" s="35" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H48" s="35"/>
       <c r="I48" s="67" t="s">
@@ -7391,17 +7349,17 @@
         <v>86</v>
       </c>
       <c r="C49" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="70" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F49" s="70"/>
       <c r="H49" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I49" s="9" t="s">
         <v>42</v>
@@ -7412,19 +7370,19 @@
         <v>86</v>
       </c>
       <c r="C50" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>42</v>
@@ -7435,16 +7393,16 @@
         <v>86</v>
       </c>
       <c r="C51" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="11" t="s">
@@ -7456,19 +7414,19 @@
         <v>86</v>
       </c>
       <c r="C52" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H52" s="9"/>
     </row>
@@ -7477,19 +7435,19 @@
         <v>86</v>
       </c>
       <c r="C53" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H53" s="9"/>
     </row>
@@ -7498,22 +7456,22 @@
         <v>86</v>
       </c>
       <c r="C54" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7521,22 +7479,22 @@
         <v>86</v>
       </c>
       <c r="C55" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E55" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>303</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7544,22 +7502,22 @@
         <v>86</v>
       </c>
       <c r="C56" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7567,19 +7525,19 @@
         <v>86</v>
       </c>
       <c r="C57" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>42</v>
@@ -7590,19 +7548,19 @@
         <v>86</v>
       </c>
       <c r="C58" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I58" s="11" t="s">
         <v>42</v>
@@ -7613,22 +7571,22 @@
         <v>86</v>
       </c>
       <c r="C59" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G59" s="36" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H59" s="36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7636,22 +7594,22 @@
         <v>86</v>
       </c>
       <c r="C60" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E60" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="G60" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="H60" s="36" t="s">
         <v>317</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="G60" s="36" t="s">
-        <v>318</v>
-      </c>
-      <c r="H60" s="36" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7659,22 +7617,22 @@
         <v>86</v>
       </c>
       <c r="C61" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G61" s="36" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H61" s="36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7682,22 +7640,22 @@
         <v>86</v>
       </c>
       <c r="C62" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G62" s="36" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H62" s="36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7705,22 +7663,22 @@
         <v>86</v>
       </c>
       <c r="C63" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G63" s="36" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H63" s="36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7728,22 +7686,22 @@
         <v>86</v>
       </c>
       <c r="C64" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G64" s="36" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H64" s="36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7751,16 +7709,16 @@
         <v>86</v>
       </c>
       <c r="C65" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G65" s="36" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H65" s="36"/>
       <c r="I65" s="11" t="s">
@@ -7772,19 +7730,19 @@
         <v>86</v>
       </c>
       <c r="C66" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G66" s="36" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H66" s="36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>42</v>
@@ -7795,20 +7753,20 @@
         <v>86</v>
       </c>
       <c r="C67" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D67" s="68" t="s">
         <v>10</v>
       </c>
       <c r="E67" s="70" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F67" s="67"/>
       <c r="G67" s="35" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>42</v>
@@ -7819,23 +7777,23 @@
         <v>86</v>
       </c>
       <c r="C68" s="67" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D68" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E68" s="70" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F68" s="70"/>
       <c r="G68" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="128" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7843,23 +7801,23 @@
         <v>86</v>
       </c>
       <c r="C69" s="67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E69" s="71" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F69" s="71"/>
       <c r="G69" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="70" s="72" customFormat="true" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7867,22 +7825,22 @@
         <v>86</v>
       </c>
       <c r="C70" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D70" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E70" s="70" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F70" s="70" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="I70" s="9"/>
     </row>
@@ -7891,7 +7849,7 @@
         <v>86</v>
       </c>
       <c r="C71" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D71" s="11" t="s">
         <v>10</v>
@@ -7903,10 +7861,10 @@
         <v>68</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H71" s="36" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I71" s="11"/>
     </row>
@@ -7915,22 +7873,22 @@
         <v>86</v>
       </c>
       <c r="C72" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D72" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H72" s="36" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7938,7 +7896,7 @@
         <v>86</v>
       </c>
       <c r="C73" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>10</v>
@@ -7950,10 +7908,10 @@
         <v>73</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H73" s="36" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7961,22 +7919,22 @@
         <v>86</v>
       </c>
       <c r="C74" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H74" s="36" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="75" s="72" customFormat="true" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7984,22 +7942,22 @@
         <v>86</v>
       </c>
       <c r="C75" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D75" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="H75" s="36" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="I75" s="11"/>
     </row>
@@ -8008,7 +7966,7 @@
         <v>86</v>
       </c>
       <c r="C76" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D76" s="11" t="s">
         <v>10</v>
@@ -8020,10 +7978,10 @@
         <v>52</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H76" s="36" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I76" s="11"/>
     </row>
@@ -8032,7 +7990,7 @@
         <v>86</v>
       </c>
       <c r="C77" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D77" s="11" t="s">
         <v>10</v>
@@ -8044,10 +8002,10 @@
         <v>63</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H77" s="36" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8055,22 +8013,22 @@
         <v>86</v>
       </c>
       <c r="C78" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D78" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H78" s="36" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8078,20 +8036,20 @@
         <v>86</v>
       </c>
       <c r="C79" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D79" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="67" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F79" s="67" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G79" s="35"/>
       <c r="H79" s="36" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8099,20 +8057,20 @@
         <v>86</v>
       </c>
       <c r="C80" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D80" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E80" s="67" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F80" s="67" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G80" s="35"/>
       <c r="H80" s="36" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8120,22 +8078,22 @@
         <v>86</v>
       </c>
       <c r="C81" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D81" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E81" s="67" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F81" s="67" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G81" s="35" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H81" s="36" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8143,22 +8101,22 @@
         <v>86</v>
       </c>
       <c r="C82" s="67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D82" s="67" t="s">
         <v>10</v>
       </c>
       <c r="E82" s="67" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F82" s="67" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G82" s="35" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H82" s="36" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8166,16 +8124,16 @@
         <v>91</v>
       </c>
       <c r="C83" s="67" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D83" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="11" t="s">
@@ -8187,16 +8145,16 @@
         <v>91</v>
       </c>
       <c r="C84" s="67" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H84" s="9"/>
       <c r="I84" s="11" t="s">
@@ -8208,16 +8166,16 @@
         <v>91</v>
       </c>
       <c r="C85" s="67" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D85" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H85" s="9"/>
       <c r="I85" s="11" t="s">
@@ -8229,17 +8187,17 @@
         <v>91</v>
       </c>
       <c r="C86" s="67" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D86" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E86" s="70" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F86" s="70"/>
       <c r="G86" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H86" s="9"/>
       <c r="I86" s="11" t="s">
@@ -8251,16 +8209,16 @@
         <v>91</v>
       </c>
       <c r="C87" s="67" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D87" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H87" s="9"/>
       <c r="I87" s="11" t="s">
@@ -8272,16 +8230,16 @@
         <v>91</v>
       </c>
       <c r="C88" s="67" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H88" s="9"/>
       <c r="I88" s="11" t="s">
@@ -8293,16 +8251,16 @@
         <v>91</v>
       </c>
       <c r="C89" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H89" s="9"/>
       <c r="I89" s="11" t="s">
@@ -8314,19 +8272,19 @@
         <v>91</v>
       </c>
       <c r="C90" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H90" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I90" s="11" t="s">
         <v>42</v>
@@ -8337,19 +8295,19 @@
         <v>91</v>
       </c>
       <c r="C91" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D91" s="68" t="s">
         <v>10</v>
       </c>
       <c r="E91" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="G91" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="H91" s="9" t="s">
         <v>388</v>
-      </c>
-      <c r="G91" s="36" t="s">
-        <v>389</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>387</v>
       </c>
       <c r="I91" s="11" t="s">
         <v>42</v>
@@ -8360,19 +8318,19 @@
         <v>91</v>
       </c>
       <c r="C92" s="67" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D92" s="68" t="s">
         <v>10</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G92" s="36" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H92" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I92" s="11" t="s">
         <v>42</v>
@@ -8389,10 +8347,10 @@
         <v>6</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G93" s="36" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H93" s="9"/>
       <c r="I93" s="11" t="s">
@@ -8410,10 +8368,10 @@
         <v>6</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G94" s="36" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H94" s="9"/>
       <c r="I94" s="11" t="s">
@@ -8431,10 +8389,10 @@
         <v>6</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G95" s="36" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H95" s="9"/>
       <c r="I95" s="11" t="s">
@@ -8452,10 +8410,10 @@
         <v>6</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G96" s="36" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H96" s="9"/>
       <c r="I96" s="11" t="s">
@@ -8473,10 +8431,10 @@
         <v>6</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G97" s="36" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H97" s="9"/>
       <c r="I97" s="11" t="s">
@@ -8494,10 +8452,10 @@
         <v>6</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H98" s="9"/>
       <c r="I98" s="11" t="s">
@@ -8509,16 +8467,16 @@
         <v>91</v>
       </c>
       <c r="C99" s="67" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D99" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H99" s="9"/>
       <c r="I99" s="11" t="s">
@@ -8530,20 +8488,20 @@
         <v>91</v>
       </c>
       <c r="C100" s="67" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D100" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E100" s="67" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F100" s="67"/>
       <c r="G100" s="35" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H100" s="35" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I100" s="67" t="s">
         <v>42</v>
@@ -8560,14 +8518,14 @@
         <v>6</v>
       </c>
       <c r="E101" s="67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F101" s="67"/>
       <c r="G101" s="35" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H101" s="35" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I101" s="67" t="s">
         <v>42</v>
@@ -8584,14 +8542,14 @@
         <v>6</v>
       </c>
       <c r="E102" s="67" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F102" s="67"/>
       <c r="G102" s="35" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H102" s="35" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I102" s="67" t="s">
         <v>42</v>
@@ -8608,14 +8566,14 @@
         <v>6</v>
       </c>
       <c r="E103" s="67" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F103" s="67"/>
       <c r="G103" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="H103" s="35" t="s">
         <v>399</v>
-      </c>
-      <c r="H103" s="35" t="s">
-        <v>398</v>
       </c>
       <c r="I103" s="67" t="s">
         <v>42</v>
@@ -8632,14 +8590,14 @@
         <v>6</v>
       </c>
       <c r="E104" s="67" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F104" s="67"/>
       <c r="G104" s="35" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H104" s="35" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I104" s="67" t="s">
         <v>42</v>
@@ -8650,17 +8608,17 @@
         <v>38</v>
       </c>
       <c r="C105" s="67" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D105" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E105" s="67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F105" s="67"/>
       <c r="G105" s="35" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H105" s="35"/>
       <c r="I105" s="67" t="s">
@@ -8672,20 +8630,20 @@
         <v>38</v>
       </c>
       <c r="C106" s="67" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D106" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E106" s="67" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F106" s="67"/>
       <c r="G106" s="35" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H106" s="35" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I106" s="67" t="s">
         <v>42</v>
@@ -8696,17 +8654,17 @@
         <v>38</v>
       </c>
       <c r="C107" s="67" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D107" s="67" t="s">
         <v>6</v>
       </c>
       <c r="E107" s="67" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F107" s="67"/>
       <c r="G107" s="35" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H107" s="35"/>
       <c r="I107" s="67" t="s">
@@ -8724,11 +8682,11 @@
         <v>6</v>
       </c>
       <c r="E108" s="67" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F108" s="67"/>
       <c r="G108" s="35" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H108" s="35"/>
       <c r="I108" s="67" t="s">
@@ -8746,11 +8704,11 @@
         <v>6</v>
       </c>
       <c r="E109" s="67" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F109" s="67"/>
       <c r="G109" s="35" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H109" s="35"/>
       <c r="I109" s="67" t="s">
@@ -8768,11 +8726,11 @@
         <v>6</v>
       </c>
       <c r="E110" s="67" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F110" s="67"/>
       <c r="G110" s="35" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H110" s="35"/>
       <c r="I110" s="67" t="s">
@@ -8790,11 +8748,11 @@
         <v>6</v>
       </c>
       <c r="E111" s="67" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F111" s="67"/>
       <c r="G111" s="35" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H111" s="35"/>
       <c r="I111" s="67" t="s">
@@ -8806,19 +8764,19 @@
         <v>38</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G112" s="36" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H112" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I112" s="11" t="s">
         <v>42</v>
@@ -8829,19 +8787,19 @@
         <v>38</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G113" s="36" t="s">
         <v>417</v>
       </c>
       <c r="H113" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I113" s="11" t="s">
         <v>42</v>
@@ -8852,19 +8810,19 @@
         <v>38</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D114" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G114" s="36" t="s">
         <v>418</v>
       </c>
       <c r="H114" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I114" s="11" t="s">
         <v>42</v>
@@ -8875,19 +8833,19 @@
         <v>38</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D115" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G115" s="36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H115" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I115" s="11" t="s">
         <v>42</v>
@@ -8898,19 +8856,19 @@
         <v>38</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D116" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G116" s="36" t="s">
         <v>419</v>
       </c>
       <c r="H116" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I116" s="11" t="s">
         <v>42</v>
@@ -8927,13 +8885,13 @@
         <v>6</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G117" s="36" t="s">
         <v>421</v>
       </c>
       <c r="H117" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>42</v>
@@ -8950,7 +8908,7 @@
         <v>6</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G118" s="9" t="s">
         <v>423</v>
@@ -8973,7 +8931,7 @@
         <v>6</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G119" s="9" t="s">
         <v>425</v>
@@ -8990,13 +8948,13 @@
         <v>38</v>
       </c>
       <c r="C120" s="67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D120" s="68" t="s">
         <v>6</v>
       </c>
       <c r="E120" s="68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G120" s="36" t="s">
         <v>427</v>
@@ -9011,7 +8969,7 @@
         <v>38</v>
       </c>
       <c r="C121" s="67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D121" s="68" t="s">
         <v>6</v>
@@ -9032,13 +8990,13 @@
         <v>38</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D122" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G122" s="9" t="s">
         <v>430</v>
@@ -9053,13 +9011,13 @@
         <v>38</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D123" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G123" s="9" t="s">
         <v>431</v>
@@ -9077,7 +9035,7 @@
         <v>6</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G124" s="9" t="s">
         <v>432</v>
@@ -9234,7 +9192,7 @@
         <v>434</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D3" s="74" t="s">
         <v>435</v>
@@ -9476,19 +9434,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C18" s="82" t="s">
         <v>471</v>
       </c>
       <c r="G18" s="81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H18" s="83" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I18" s="82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L18" s="44"/>
     </row>
@@ -9560,19 +9518,19 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C25" s="82" t="s">
         <v>474</v>
       </c>
       <c r="G25" s="81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H25" s="83" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I25" s="82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9653,7 +9611,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C33" s="83" t="s">
         <v>477</v>
@@ -9665,13 +9623,13 @@
         <v>479</v>
       </c>
       <c r="G33" s="81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H33" s="83" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I33" s="82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9781,7 +9739,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="44" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>486</v>

</xml_diff>